<commit_message>
Se acaba el plan de calidad
</commit_message>
<xml_diff>
--- a/Plan de Calidad Ivan Ruiz.xlsx
+++ b/Plan de Calidad Ivan Ruiz.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan0\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan0\Downloads\ApiRestGitHub\retoQaDevOps2023C1G1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF8683A-9007-4AB0-932A-D94C30E5518E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B663EA-FF10-4135-92CE-D8A04B8A300A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="322" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Calidad - Grupo 1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Plan de calidad</t>
   </si>
@@ -59,27 +59,6 @@
   </si>
   <si>
     <t>Equipo 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cristhian Moreno Garzón
-Gretty María Mosquera Taborda
-Ivan Dario Ruiz Bernal
-Jesús Miguel Molina Mendoza
-Jessica Andrea López Obando
-Melissa Meneses Acevedo
-Nevardo Antonio Ospina Zuñiga
-Sergio Andrés Balcázar Restrepo
-Yeison Ferney Osorio Buitrago
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Se requiere verificar el funcionamiento de servicios tipo Soap y Rest para un total de 36 peticiones.
-Probar un servicio se debe a varios factores como el de garantizar que el servicio esté funcionando correctamente y devolviendo los datos esperados. Esto implica asegurarse de que la petición sea correcta y que la respuesta del servidor sea la adecuada.
-</t>
-  </si>
-  <si>
-    <t>El alcance de las pruebas se limitan a la funcionalidad especifica de cada servicio realizando pruebas funcionales automatizadas, comprobando que las peticiones realizadas funcionen correctamente.
-El alcance de las pruebas cubre la verificación de que se manejen adecuadamente situaciones de éxito y errores.</t>
   </si>
   <si>
     <t xml:space="preserve">Queda fuera del alcance funcionalidades que no están comprometidas dentro del alcance, tales como:
@@ -110,12 +89,48 @@
     <t xml:space="preserve">
 </t>
   </si>
+  <si>
+    <t>Ivan Dario Ruiz Bernal</t>
+  </si>
+  <si>
+    <t>Equipo 2</t>
+  </si>
+  <si>
+    <t>Equipo 3</t>
+  </si>
+  <si>
+    <t>Equipo 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se requiere verificar el funcionamiento del servicio tipo Soap suma
+Probar un servicio se debe a varios factores como el de garantizar que el servicio esté funcionando correctamente y devolviendo los datos esperados. Esto implica asegurarse de que la petición sea correcta y que la respuesta del servidor sea la adecuada.
+</t>
+  </si>
+  <si>
+    <t>El alcance de las pruebas se limitan a la funcionalidad especifica del servicio realizando pruebas funcionales automatizadas, comprobando que las peticiones realizadas funcionen correctamente.
+El alcance de las pruebas cubre la verificación de que se manejen adecuadamente situaciones de éxito y cuando es posible errores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se requiere verificar el funcionamiento del servicio tipo Soap cambio de divisas
+Probar un servicio se debe a varios factores como el de garantizar que el servicio esté funcionando correctamente y devolviendo los datos esperados. Esto implica asegurarse de que la petición sea correcta y que la respuesta del servidor sea la adecuada.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se requiere verificar el funcionamiento del servicio tipo Rest actualización de comentarios
+Probar un servicio se debe a varios factores como el de garantizar que el servicio esté funcionando correctamente y devolviendo los datos esperados. Esto implica asegurarse de que la petición sea correcta y que la respuesta del servidor sea la adecuada.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se requiere verificar el funcionamiento del servicio tipo Rest eliminar un post
+Probar un servicio se debe a varios factores como el de garantizar que el servicio esté funcionando correctamente y devolviendo los datos esperados. Esto implica asegurarse de que la petición sea correcta y que la respuesta del servidor sea la adecuada.
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -143,6 +158,11 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -207,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -224,9 +244,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -493,8 +510,8 @@
   </sheetPr>
   <dimension ref="A1:Y12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -510,18 +527,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="51.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:25">
       <c r="A2" s="2" t="s">
@@ -570,7 +587,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" spans="1:25" ht="199.5">
+    <row r="3" spans="1:25" ht="191.25">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -578,28 +595,28 @@
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
@@ -617,11 +634,101 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="5" spans="1:25" ht="12.75">
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:25" ht="12.75">
-      <c r="H6" s="7"/>
+    <row r="4" spans="1:25" ht="199.5">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="199.5">
+      <c r="A5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="191.25">
+      <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:25" ht="12.75">
       <c r="C7" s="1"/>
@@ -630,8 +737,8 @@
       <c r="C8" s="1"/>
     </row>
     <row r="10" spans="1:25" ht="14.25">
-      <c r="C10" s="8" t="s">
-        <v>21</v>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="12.75">
@@ -641,6 +748,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>

</xml_diff>